<commit_message>
updated for new messages
</commit_message>
<xml_diff>
--- a/references/MessagePayloadBlockFormatter.xlsx
+++ b/references/MessagePayloadBlockFormatter.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1920" uniqueCount="774">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="777">
   <si>
     <t>Start</t>
   </si>
@@ -2344,6 +2344,15 @@
   </si>
   <si>
     <t>Group Assignment Control</t>
+  </si>
+  <si>
+    <t>Single Slot Binary Message</t>
+  </si>
+  <si>
+    <t>Multiple Slot Binary Message with Communitation State</t>
+  </si>
+  <si>
+    <t>Long-range Automatic Identification System Broadcast Message</t>
   </si>
 </sst>
 </file>
@@ -2508,7 +2517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -2541,8 +2550,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2914,8 +2921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M450"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A342" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A344" sqref="A344"/>
+    <sheetView tabSelected="1" topLeftCell="A391" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C428" sqref="C428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13109,10 +13116,10 @@
       <c r="M342" s="4"/>
     </row>
     <row r="343" spans="1:13">
-      <c r="A343" s="24" t="s">
+      <c r="A343" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B343" s="25" t="s">
+      <c r="B343" s="19" t="s">
         <v>355</v>
       </c>
       <c r="C343" s="1" t="s">
@@ -13729,10 +13736,10 @@
       <c r="M362" s="4"/>
     </row>
     <row r="363" spans="1:13">
-      <c r="A363" s="4" t="s">
+      <c r="A363" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B363" s="1" t="s">
+      <c r="B363" s="19" t="s">
         <v>392</v>
       </c>
       <c r="C363" s="1" t="s">
@@ -14770,6 +14777,9 @@
       <c r="B397" s="1" t="s">
         <v>429</v>
       </c>
+      <c r="C397" s="1" t="s">
+        <v>774</v>
+      </c>
       <c r="E397" s="4"/>
       <c r="F397" s="4"/>
       <c r="G397" s="4"/>
@@ -15117,6 +15127,9 @@
       <c r="B409" s="1" t="s">
         <v>440</v>
       </c>
+      <c r="C409" s="1" t="s">
+        <v>775</v>
+      </c>
       <c r="E409" s="4"/>
       <c r="F409" s="4"/>
       <c r="G409" s="4"/>
@@ -15321,7 +15334,7 @@
       <c r="H415" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="I415" t="str">
+      <c r="I415" s="20" t="str">
         <f t="shared" si="73"/>
         <v>messageBlocks.add(new PayloadBlock(40, 69, 30, "Destination MMSI", "dest_mmsi", "u", "Message destination"));</v>
       </c>
@@ -15353,7 +15366,7 @@
       <c r="H416" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="I416" t="str">
+      <c r="I416" s="20" t="str">
         <f t="shared" si="73"/>
         <v>messageBlocks.add(new PayloadBlock(70, 71, 2, "Spare", "", "x", "Byte Alignment"));</v>
       </c>
@@ -15667,6 +15680,9 @@
       </c>
       <c r="B427" s="1" t="s">
         <v>451</v>
+      </c>
+      <c r="C427" s="1" t="s">
+        <v>776</v>
       </c>
       <c r="E427" s="4"/>
       <c r="F427" s="4"/>

</xml_diff>